<commit_message>
🔄 Actualización automática del mapa (mapa_interactivo_AYKO.html)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:P92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2318,7 +2318,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>803608331</t>
+          <t>803608455</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2328,7 +2328,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 4875</t>
+          <t>VALDENEGRO /ALT/ 4037</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>803608331</t>
+          <t>803608455</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna terminal168 con rienda a pique fuera de plomo  y base con cimentación rota </t>
+          <t>Cambiar poste podrido apoyado en tanque de agua. Es sobre parque junto a medianera.  Dar prioridad .</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2371,18 +2371,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.484493</v>
+        <v>-58.493679</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.572049</v>
+        <v>-34.557149</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2394,7 +2394,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>803608455</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2404,17 +2404,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>VALDENEGRO /ALT/ 4037</t>
+          <t>COCHABAMBA /ALT/ 1790</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>803608455</t>
+          <t>803608463</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Cambiar poste podrido apoyado en tanque de agua. Es sobre parque junto a medianera.  Dar prioridad .</t>
+          <t>SIN RIEGO</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2442,55 +2442,55 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.493679</v>
+        <v>-58.391153</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.557149</v>
+        <v>-34.624022</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>-281</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2/24/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>COCHABAMBA /ALT/ 1790</t>
+          <t>SOLER /ALT/ 4517</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803608463</t>
+          <t>803651203</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>SIN RIEGO</t>
+          <t>columna de 114 con nodo y redes nuestra.</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2527,14 +2527,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.391153</v>
+        <v>-58.423405</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.624022</v>
+        <v>-34.588075</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2546,17 +2546,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-281</t>
+          <t>-307</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>SOLER /ALT/ 4517</t>
+          <t>BERUTI ANTONIO /ALT/ 4645</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>803651203</t>
+          <t>804288212</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2581,11 +2581,11 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>columna de 114 con nodo y redes nuestra.</t>
+          <t>Picada traspasar red y retirar columna</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2594,19 +2594,19 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.423405</v>
+        <v>-58.42486</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.588075</v>
+        <v>-34.577318</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -2622,27 +2622,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-307</t>
+          <t>-316</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>4/3/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>BERUTI ANTONIO /ALT/ 4645</t>
+          <t>ALBERTI /ALT/ 621</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804288212</t>
+          <t>804468365</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2657,7 +2657,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada traspasar red y retirar columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2675,18 +2675,18 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.42486</v>
+        <v>-58.401202</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.577318</v>
+        <v>-34.61683</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2698,27 +2698,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-316</t>
+          <t>-326</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4/3/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ALBERTI /ALT/ 621</t>
+          <t>GARCIA DEL RIO /ALT/ 3354</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804468365</t>
+          <t>804634199</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2733,7 +2733,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar poste de vereda. Reparar la vereda donde estaba colocado el poste.</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2751,30 +2751,30 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.401202</v>
+        <v>-58.478106</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.61683</v>
+        <v>-34.551523</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-326</t>
+          <t>-327</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2784,7 +2784,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>GARCIA DEL RIO /ALT/ 3354</t>
+          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804634199</t>
+          <t>804634203</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Retirar poste de vereda. Reparar la vereda donde estaba colocado el poste.</t>
+          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2817,28 +2817,28 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.478106</v>
+        <v>-58.491074</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.551523</v>
+        <v>-34.575623</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2850,7 +2850,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-327</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2860,17 +2860,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ROOSEVELT F D ,AV. /ALT/ 5439</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804634203</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Colocar columna R200 y  dar aviso para el traspaso de nodos. (TECO y TLC)</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2893,12 +2893,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2907,14 +2907,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.491074</v>
+        <v>-58.525125</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.575623</v>
+        <v>-34.604668</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2926,27 +2926,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5572</t>
+          <t>-336</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SANABRIA 4289</t>
+          <t>BAUNESS /ALT/ 1419</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804663652</t>
+          <t>804838856</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>"Aplomar columna 114 con rienda a pique o colocar terminal"</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2979,14 +2979,14 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.516755</v>
+        <v>-58.479168</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.6002</v>
+        <v>-34.584482</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3002,27 +3002,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>-338</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>PARAGUAY /ALT/ 4283</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804838861</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3059,46 +3059,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.525125</v>
+        <v>-58.421964</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.604668</v>
+        <v>-34.586342</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5574</t>
+          <t>-339</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/21/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>GRIVEO 3909</t>
+          <t>GRIVEO /ALT/ 2435</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804663683</t>
+          <t>804838868</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Poste Inclinado</t>
+          <t xml:space="preserve">Aplomar columna 114  </t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3131,14 +3131,14 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.517126</v>
+        <v>-58.498493</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.592774</v>
+        <v>-34.581262</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3154,7 +3154,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-336</t>
+          <t>-340</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3164,17 +3164,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>BAUNESS /ALT/ 1419</t>
+          <t>SUPERI /ALT/ 1445</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804838856</t>
+          <t>804838869</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>"Aplomar columna 114 con rienda a pique o colocar terminal"</t>
+          <t>Columna podrida en la base</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3211,14 +3211,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.479168</v>
+        <v>-58.460666</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.584482</v>
+        <v>-34.573823</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3230,7 +3230,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>-341</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3240,17 +3240,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 4283</t>
+          <t>3 DE FEBRERO /ALT/ 4835</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804838861</t>
+          <t>804838980</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3265,7 +3265,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>"Retirar poste teco cobre en desuso entrada Edificio reclamo municipal "</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3283,40 +3283,40 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.421964</v>
+        <v>-58.469157</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.586342</v>
+        <v>-34.536783</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-339</t>
+          <t>-342</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>GRIVEO /ALT/ 2435</t>
+          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804838868</t>
+          <t>804839148</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3341,15 +3341,15 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114  </t>
+          <t>Cambiar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3363,10 +3363,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.498493</v>
+        <v>-58.502447</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.581262</v>
+        <v>-34.561008</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3382,27 +3382,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-340</t>
+          <t>-344</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SUPERI /ALT/ 1445</t>
+          <t>ANDONAEGUI /ALT/ 1690</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804838869</t>
+          <t>804839162</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3417,15 +3417,15 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Columna podrida en la base</t>
+          <t>Aplomar columna de 114. - VIRARDI</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3439,14 +3439,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.460666</v>
+        <v>-58.483947</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.573823</v>
+        <v>-34.583207</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3458,27 +3458,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-341</t>
+          <t>-346</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/21/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO /ALT/ 4835</t>
+          <t>ARGERICH /ALT/ 4710</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804838980</t>
+          <t>804839198</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3493,15 +3493,15 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>"Retirar poste teco cobre en desuso entrada Edificio reclamo municipal "</t>
+          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3515,14 +3515,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.469157</v>
+        <v>-58.503673</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.536783</v>
+        <v>-34.586925</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3534,7 +3534,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-342</t>
+          <t>-347</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3544,17 +3544,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>WILLIAMS ALBERTO /ALT/ 5625</t>
+          <t>AVALOS /ALT/ 1610</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804839148</t>
+          <t>804839214</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. - VIRARDI</t>
+          <t>Cambiar columna de 168 - VIRARDI</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3582,7 +3582,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente TLC</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3591,10 +3591,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.502447</v>
+        <v>-58.480099</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.561008</v>
+        <v>-34.582085</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3610,7 +3610,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-344</t>
+          <t>-353</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3620,17 +3620,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1690</t>
+          <t>CAAGUAZU /ALT/ 5703</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804839162</t>
+          <t>804839589</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114. - VIRARDI</t>
+          <t>Cambiar columna de 114. Fuera de plomo empotrada en árbol colocar rienda. ( se pasa tareas a contratista tratista de limpieza tensado y elevación del tendido).  - VIRARDI</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3667,14 +3667,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.483947</v>
+        <v>-58.511462</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.583207</v>
+        <v>-34.640542</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3686,7 +3686,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-345</t>
+          <t>-354</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3696,17 +3696,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ANDONAEGUI /ALT/ 1774</t>
+          <t>CONDARCO /ALT/ 5316</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804839181</t>
+          <t>804839626</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Aplomo/cambio de columna de 168 colocar columna y rienda en norma.  - VIRARDI</t>
+          <t>Aplomo de columna de PRFV - VIRARDI</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3743,10 +3743,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.484513</v>
+        <v>-58.504455</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.582786</v>
+        <v>-34.579941</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3762,7 +3762,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-346</t>
+          <t>-355</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ARGERICH /ALT/ 4710</t>
+          <t>CUENCA /ALT/ 4480</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3782,7 +3782,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804839198</t>
+          <t>804839675</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cambiar poste con rienda podrido en su base - VIRARDI</t>
+          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3805,24 +3805,24 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente TLC</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.503673</v>
+        <v>-58.504568</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.586925</v>
+        <v>-34.590534</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-347</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3848,17 +3848,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>AVALOS /ALT/ 1610</t>
+          <t>CABEZON JOSE LEON /ALT/ 2714</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804839214</t>
+          <t>804839875</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar columna de 168 - VIRARDI</t>
+          <t>Aplomo de columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3881,12 +3881,12 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo/Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3895,10 +3895,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.480099</v>
+        <v>-58.503195</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.582085</v>
+        <v>-34.581735</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3914,7 +3914,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-353</t>
+          <t>-363</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3924,17 +3924,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>CAAGUAZU /ALT/ 5703</t>
+          <t>OSLO /ALT/ 1255</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804839589</t>
+          <t>804839962</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar columna de 114. Fuera de plomo empotrada en árbol colocar rienda. ( se pasa tareas a contratista tratista de limpieza tensado y elevación del tendido).  - VIRARDI</t>
+          <t>Cambiar columna de 168 podrida en su base.  - VIRARDI</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3971,14 +3971,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.511462</v>
+        <v>-58.481767</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.640542</v>
+        <v>-34.589507</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3990,7 +3990,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-354</t>
+          <t>-364</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>CONDARCO /ALT/ 5316</t>
+          <t>PAROISSIEN /ALT/ 4871</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4010,7 +4010,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>804839626</t>
+          <t>804839991</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4025,7 +4025,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Aplomo de columna de PRFV - VIRARDI</t>
+          <t>Aplomar columna de 114 - VIRARDI</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4047,14 +4047,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.504455</v>
+        <v>-58.493164</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.579941</v>
+        <v>-34.55732</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4066,7 +4066,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-355</t>
+          <t>-365</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4076,7 +4076,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CUENCA /ALT/ 4480</t>
+          <t>QUESADA /ALT/ 5290</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>804839675</t>
+          <t>804839995</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna nueva fuera de plomo sostiene nodo de Telecentro.  Reclamo municipal.  - VIRARDI</t>
+          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4109,12 +4109,12 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Nodo/Fuente TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4123,10 +4123,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.504568</v>
+        <v>-58.491934</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.590534</v>
+        <v>-34.569348</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4142,7 +4142,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-356</t>
+          <t>-366</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4152,7 +4152,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CUENCA /ALT/ 4845</t>
+          <t>QUESADA /ALT/ 6088</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4162,7 +4162,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>804839715</t>
+          <t>804840016</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4177,7 +4177,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Retiro de poste viejo en desuso liberado podrido en su base.  - VIRARDI</t>
+          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4185,7 +4185,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4195,14 +4195,14 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.507182</v>
+        <v>-58.501418</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.58749</v>
+        <v>-34.574363</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4218,7 +4218,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-359</t>
+          <t>-367</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4228,7 +4228,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>CABEZON JOSE LEON /ALT/ 2714</t>
+          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>804839875</t>
+          <t>804840024</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4275,14 +4275,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.503195</v>
+        <v>-58.494584</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.581735</v>
+        <v>-34.554981</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4294,27 +4294,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-363</t>
+          <t>-368</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>OSLO /ALT/ 1255</t>
+          <t>ARIAS /ALT/ 1620</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>804839962</t>
+          <t>804876039</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4329,15 +4329,15 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Cambiar columna de 168 podrida en su base.  - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4347,18 +4347,18 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.481767</v>
+        <v>-58.465608</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.589507</v>
+        <v>-34.538489</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4370,27 +4370,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-364</t>
+          <t>-372</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>PAROISSIEN /ALT/ 4871</t>
+          <t>CAMARGO /ALT/ 25</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>804839991</t>
+          <t>804903809</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4405,15 +4405,15 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Aplomar columna de 114 - VIRARDI</t>
+          <t>Aplomar columna 114 con rienda a pique</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4427,14 +4427,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.493164</v>
+        <v>-58.436788</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.55732</v>
+        <v>-34.604014</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4446,27 +4446,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-365</t>
+          <t>-373</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 5290</t>
+          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>804839995</t>
+          <t>804903810</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4481,15 +4481,15 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Columna nueva de PVC fuera de plomo.  - VIRARDI</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4503,46 +4503,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.491934</v>
+        <v>-58.439461</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.569348</v>
+        <v>-34.605744</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-366</t>
+          <t>-375</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>QUESADA /ALT/ 6088</t>
+          <t>PAVON /ALT/ 3335</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>804840016</t>
+          <t>804903824</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4557,15 +4557,15 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 cambiar rienda.  - VIRARDI</t>
+          <t>Colocar columna nueva donde estaba la anterior cortada</t>
         </is>
       </c>
       <c r="I55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4579,46 +4579,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.501418</v>
+        <v>-58.412418</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.574363</v>
+        <v>-34.629288</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-367</t>
+          <t>-376</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>RUIZ HUIDOBRO ,AV. /ALT/ 4771</t>
+          <t xml:space="preserve"> Valentin Gomez 3803</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>804840024</t>
+          <t>804903787</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4633,15 +4633,15 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Aplomo de columna de 114 - VIRARDI</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4655,46 +4655,46 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.494584</v>
+        <v>-58.418424</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.554981</v>
+        <v>-34.604463</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-368</t>
+          <t>-377</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ARIAS /ALT/ 1620</t>
+          <t>HUMAHUACA /ALT/ 3918</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>804876039</t>
+          <t>804903788</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda </t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4717,7 +4717,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4727,50 +4727,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.465608</v>
+        <v>-58.419694</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.538489</v>
+        <v>-34.602062</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-372</t>
+          <t>-383</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CAMARGO /ALT/ 25</t>
+          <t>VALDERRAMA /ALT/ 4187</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>804903809</t>
+          <t>805507401</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar columna 114 con rienda a pique</t>
+          <t xml:space="preserve">Aplomar columna 114 </t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4807,14 +4807,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.436788</v>
+        <v>-58.481834</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.604014</v>
+        <v>-34.560796</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4826,27 +4826,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-373</t>
+          <t>-384</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>GALLARDO ANGEL ,AV. /ALT/ 608</t>
+          <t>LUGONES 1721</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>804903810</t>
+          <t>805507408</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4883,46 +4883,46 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.439461</v>
+        <v>-58.473936</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.605744</v>
+        <v>-34.577346</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-375</t>
+          <t>-385</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>PAVON /ALT/ 3335</t>
+          <t>MOLDES /ALT/ 1913</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>804903824</t>
+          <t>805507415</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Colocar columna nueva donde estaba la anterior cortada</t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4959,46 +4959,46 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.412418</v>
+        <v>-58.45789</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.629288</v>
+        <v>-34.565423</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-376</t>
+          <t>-386</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valentin Gomez 3803</t>
+          <t>MOLDES /ALT/ 1943</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>804903787</t>
+          <t>805507419</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5013,7 +5013,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5021,12 +5021,12 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -5035,46 +5035,46 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.418424</v>
+        <v>-58.458217</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.604463</v>
+        <v>-34.565043</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-377</t>
+          <t>-391</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>HUMAHUACA /ALT/ 3918</t>
+          <t>IBERA /ALT/ 5074</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>804903788</t>
+          <t>805676610</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5089,7 +5089,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5111,46 +5111,46 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.419694</v>
+        <v>-58.49045</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.602062</v>
+        <v>-34.566894</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-383</t>
+          <t>-392</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>VALDERRAMA /ALT/ 4187</t>
+          <t>GARCIA TEODORO /ALT/ 1775</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>805507401</t>
+          <t>805676615</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5165,7 +5165,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 114 </t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5173,7 +5173,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5187,14 +5187,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.481834</v>
+        <v>-58.440367</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.560796</v>
+        <v>-34.563551</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5206,27 +5206,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-384</t>
+          <t>-393</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/5/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>LUGONES 1721</t>
+          <t>3 DE FEBRERO /ALT/ 1272</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>805507408</t>
+          <t>805676618</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5241,7 +5241,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Aplomar columna 168 - La columna esta frente a la altura 1721</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5249,7 +5249,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5263,10 +5263,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.473936</v>
+        <v>-58.445186</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.577346</v>
+        <v>-34.567417</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5282,27 +5282,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-385</t>
+          <t>-395</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1913</t>
+          <t>POSADAS 1567</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>805507415</t>
+          <t>805707278</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5317,7 +5317,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5325,7 +5325,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5339,36 +5339,36 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.45789</v>
+        <v>-58.387847</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.565423</v>
+        <v>-34.587043</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-386</t>
+          <t>-403</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>MOLDES /ALT/ 1943</t>
+          <t>SUCRE MRCAL A J DE /ALT/ 3515</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5378,7 +5378,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>805507419</t>
+          <t>805722878</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Dos columnas fuera de plomo - aplomar o cambiar la que no tiene nodo de TLC</t>
+          <t xml:space="preserve">Retirar poste teco cobre tirado y reparar vereda </t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5401,24 +5401,24 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.458217</v>
+        <v>-58.466241</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.565043</v>
+        <v>-34.57047</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5434,27 +5434,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-391</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>IBERA /ALT/ 5074</t>
+          <t>Amenabar 3048</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>805676610</t>
+          <t>805791896</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5469,7 +5469,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5477,7 +5477,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5491,14 +5491,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.49045</v>
+        <v>-58.46579</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.566894</v>
+        <v>-34.555012</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5510,27 +5510,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-392</t>
+          <t>-405</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>GARCIA TEODORO /ALT/ 1775</t>
+          <t>Arcos 1855</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>805676615</t>
+          <t>805791908</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5545,7 +5545,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5567,10 +5567,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.440367</v>
+        <v>-58.451835</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.563551</v>
+        <v>-34.562646</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5586,27 +5586,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-393</t>
+          <t>-406</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>5/5/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO /ALT/ 1272</t>
+          <t>Olof palme 4144</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>805676618</t>
+          <t>805791925</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5621,7 +5621,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Tensar 2 riendas a pique columna 168</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5629,7 +5629,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5639,18 +5639,18 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.445186</v>
+        <v>-58.488252</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.567417</v>
+        <v>-34.553391</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5662,27 +5662,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-395</t>
+          <t>-407</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>POSADAS 1567</t>
+          <t>Cabildo 4148</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>805707278</t>
+          <t>805791933</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5697,7 +5697,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5705,7 +5705,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5715,50 +5715,50 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.387847</v>
+        <v>-58.470837</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.587043</v>
+        <v>-34.545751</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-403</t>
+          <t>-408</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/8/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SUCRE MRCAL A J DE /ALT/ 3515</t>
+          <t>Larralde 2847</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>805722878</t>
+          <t>805791941</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5773,7 +5773,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Retirar poste teco cobre tirado y reparar vereda </t>
+          <t>Aplomar columna 114</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5781,28 +5781,28 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.466241</v>
+        <v>-58.472267</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.57047</v>
+        <v>-34.551163</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5814,17 +5814,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-404</t>
+          <t>-421</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Amenabar 3048</t>
+          <t>BESARES 1699</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5834,7 +5834,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>805791896</t>
+          <t>806926565</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5849,7 +5849,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5857,7 +5857,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5871,10 +5871,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.46579</v>
+        <v>-58.464144</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.555012</v>
+        <v>-34.541832</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5890,27 +5890,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-405</t>
+          <t>-425</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Arcos 1855</t>
+          <t>Av. Eva Peron 7437</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>805791908</t>
+          <t>806926621</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5925,7 +5925,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base, posee nodo propio.&lt;br&gt;</t>
+          <t>Aplomar o cambiar columna de 114</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5947,14 +5947,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.451835</v>
+        <v>-58.501029</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.562646</v>
+        <v>-34.673558</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5966,27 +5966,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-406</t>
+          <t>-426</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Olof palme 4144</t>
+          <t>Av. Eva Peron 7471</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>805791925</t>
+          <t>806926647</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6001,7 +6001,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Tensar 2 riendas a pique columna 168</t>
+          <t>Aplomar columna de 168 con rienda</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6009,7 +6009,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6023,14 +6023,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.488252</v>
+        <v>-58.501565</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.553391</v>
+        <v>-34.673845</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6042,27 +6042,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-407</t>
+          <t>-430</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Cabildo 4148</t>
+          <t>Araoz 606</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>805791933</t>
+          <t>806926712</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomar columna 168 con rienda a pique </t>
+          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6085,7 +6085,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -6095,50 +6095,50 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.470837</v>
+        <v>-58.434761</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.545751</v>
+        <v>-34.598381</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-408</t>
+          <t>-432</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>5/8/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Larralde 2847</t>
+          <t>ALVAREZ JULIAN 618</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>805791941</t>
+          <t>806926759</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Columna con base corroida sin riesgo de caida al 14/05/2025</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6161,12 +6161,12 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -6175,46 +6175,46 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.472267</v>
+        <v>-58.433867</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.551163</v>
+        <v>-34.599149</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>5805</t>
+          <t>-433</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>5/14/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>GUTENBERG 4134</t>
+          <t>Moldes 2720</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>806926378</t>
+          <t>806926767</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6229,7 +6229,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6237,7 +6237,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6251,14 +6251,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.51665</v>
+        <v>-58.464177</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.596644</v>
+        <v>-34.558239</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6270,7 +6270,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-421</t>
+          <t>-434</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6280,17 +6280,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>BESARES 1699</t>
+          <t>Billinghurst 1478</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>806926565</t>
+          <t>806926806</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6305,7 +6305,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 picada en base tener en cuenta que hay acometidas subterraneas que bajan por la columna para entrar en Libertador 8008 tanto de HFC como FTTH colocar medias cañas y colocar cerca para que quedan precintadas a la columna</t>
+          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6327,46 +6327,46 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.464144</v>
+        <v>-58.412302</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.541832</v>
+        <v>-34.59301</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-422</t>
+          <t>-448</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Franklin Roosevelt 4901</t>
+          <t>Tronador 3826</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>806926575</t>
+          <t>806975699</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6381,11 +6381,11 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Aplomar columna 114</t>
+          <t>Columna de retención (columna más ancha</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -6403,14 +6403,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.485102</v>
+        <v>-58.485056</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.572327</v>
+        <v>-34.555059</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6422,27 +6422,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-425</t>
+          <t>-450</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Av. Eva Peron 7437</t>
+          <t>Moldes 2325</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>806926621</t>
+          <t>807044059</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6457,7 +6457,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Aplomar o cambiar columna de 114</t>
+          <t xml:space="preserve">Corroida en base para cambiar contiene CDO/NAP propio </t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6479,14 +6479,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.501029</v>
+        <v>-58.461167</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.673558</v>
+        <v>-34.561613</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6498,27 +6498,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-426</t>
+          <t>-480</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Av. Eva Peron 7471</t>
+          <t>Arias 4384</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>806926647</t>
+          <t>807537909</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6533,7 +6533,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Aplomar columna de 168 con rienda</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6541,7 +6541,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6551,18 +6551,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.501565</v>
+        <v>-58.49147</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.673845</v>
+        <v>-34.55031</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6574,27 +6574,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>-430</t>
+          <t>-482</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Araoz 606</t>
+          <t>Av. Coronel Diaz 2596</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>806926712</t>
+          <t>807605730</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6607,11 +6607,7 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>columna base corroida sin riesgo de caída a la fecha. 14/05/2025</t>
-        </is>
-      </c>
+      <c r="H82" t="inlineStr"/>
       <c r="I82" t="n">
         <v>1</v>
       </c>
@@ -6631,14 +6627,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.434761</v>
+        <v>-58.405761</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.598381</v>
+        <v>-34.582476</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6650,27 +6646,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-432</t>
+          <t>-486</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>ALVAREZ JULIAN 618</t>
+          <t>Del Libertador 4596</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>806926759</t>
+          <t>807762871</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6685,7 +6681,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Columna con base corroida sin riesgo de caida al 14/05/2025</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6707,10 +6703,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.433867</v>
+        <v>-58.432241</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.599149</v>
+        <v>-34.56642</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -6726,27 +6722,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>-433</t>
+          <t>-487</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/23/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Moldes 2720</t>
+          <t>Gorriti 3735</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>806926767</t>
+          <t>807762979</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6761,7 +6757,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Poste - Pasan 5 lingas y la línea de cobre </t>
+          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6779,50 +6775,50 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.464177</v>
+        <v>-58.417348</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.558239</v>
+        <v>-34.595467</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-434</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Billinghurst 1478</t>
+          <t>ECHEANDIA 4200</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>806926806</t>
+          <t>807762996</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6837,7 +6833,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Columna base corroida con Nap y ganancias de ambas compañias, </t>
+          <t>Columna inclinada con base  corroida</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6855,18 +6851,18 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.412302</v>
+        <v>-58.472311</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.59301</v>
+        <v>-34.654867</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6878,27 +6874,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>-448</t>
+          <t>6239</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Tronador 3826</t>
+          <t>PALPA 2964</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>806975699</t>
+          <t>807763098</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6913,11 +6909,11 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Columna de retención (columna más ancha</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
@@ -6935,14 +6931,14 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.485056</v>
+        <v>-58.450113</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.555059</v>
+        <v>-34.574534</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -6954,27 +6950,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-450</t>
+          <t>-488</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Moldes 2325</t>
+          <t>Blanco Encalada 4896</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>807044059</t>
+          <t>807763099</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6989,7 +6985,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t xml:space="preserve">Corroida en base para cambiar contiene CDO/NAP propio </t>
+          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7007,18 +7003,18 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.461167</v>
+        <v>-58.484729</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.561613</v>
+        <v>-34.574614</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -7030,27 +7026,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-470</t>
+          <t>-491</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Av. Escalada 2831</t>
+          <t>3 de Febrero 2171</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>807208264</t>
+          <t>807789702</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7065,7 +7061,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 propia picada en base con NAP</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7087,46 +7083,46 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.470815</v>
+        <v>-58.452636</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.664201</v>
+        <v>-34.558607</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>-480</t>
+          <t>-500</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Arias 4384</t>
+          <t>Castañares 5656</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>807537909</t>
+          <t>807965768</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7141,7 +7137,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Columna chocada con rienda a pique</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7159,50 +7155,50 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.49147</v>
+        <v>-58.479921</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.55031</v>
+        <v>-34.673021</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>-482</t>
+          <t>6394</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Av. Coronel Diaz 2596</t>
+          <t>LAMBARE 1076</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>807605730</t>
+          <t>808194286</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -7215,7 +7211,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H90" t="inlineStr"/>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I90" t="n">
         <v>1</v>
       </c>
@@ -7235,14 +7235,14 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.405761</v>
+        <v>-58.43008</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.582476</v>
+        <v>-34.601416</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -7254,27 +7254,27 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>-486</t>
+          <t>6399</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Del Libertador 4596</t>
+          <t>ESCALADA AV. 966</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>807762871</t>
+          <t>808258198</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -7311,46 +7311,46 @@
         </is>
       </c>
       <c r="M91" t="n">
-        <v>-58.432241</v>
+        <v>-58.493069</v>
       </c>
       <c r="N91" t="n">
-        <v>-34.56642</v>
+        <v>-34.646557</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>-487</t>
+          <t>-515</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>6/23/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Gorriti 3735</t>
+          <t>Rivadavia 7470</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>807762979</t>
+          <t>808263485</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -7365,7 +7365,7 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>NAP FTTH Columna MAL ESTADO ROTA EN BASE</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I92" t="n">
@@ -7387,475 +7387,19 @@
         </is>
       </c>
       <c r="M92" t="n">
-        <v>-58.417348</v>
+        <v>-58.470715</v>
       </c>
       <c r="N92" t="n">
-        <v>-34.595467</v>
+        <v>-34.631107</v>
       </c>
       <c r="O92" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P92" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>6223</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>6/24/2025</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>ECHEANDIA 4200</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>807762996</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>Columna inclinada con base  corroida</t>
-        </is>
-      </c>
-      <c r="I93" t="n">
-        <v>1</v>
-      </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M93" t="n">
-        <v>-58.472311</v>
-      </c>
-      <c r="N93" t="n">
-        <v>-34.654867</v>
-      </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P93" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>6239</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>6/24/2025</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>PALPA 2964</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>807763098</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I94" t="n">
-        <v>1</v>
-      </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M94" t="n">
-        <v>-58.450113</v>
-      </c>
-      <c r="N94" t="n">
-        <v>-34.574534</v>
-      </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P94" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>-488</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>6/24/2025</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Blanco Encalada 4896</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>807763099</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>Pendiente traspaso rxo y retiro de columna podrida</t>
-        </is>
-      </c>
-      <c r="I95" t="n">
-        <v>1</v>
-      </c>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M95" t="n">
-        <v>-58.484729</v>
-      </c>
-      <c r="N95" t="n">
-        <v>-34.574614</v>
-      </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P95" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>-491</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>6/26/2025</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>3 de Febrero 2171</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>807789702</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Columna 114 propia picada en base con NAP</t>
-        </is>
-      </c>
-      <c r="I96" t="n">
-        <v>1</v>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M96" t="n">
-        <v>-58.452636</v>
-      </c>
-      <c r="N96" t="n">
-        <v>-34.558607</v>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P96" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>-500</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>7/3/2025</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Castañares 5656</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>807965768</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>Columna chocada con rienda a pique</t>
-        </is>
-      </c>
-      <c r="I97" t="n">
-        <v>1</v>
-      </c>
-      <c r="J97" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L97" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M97" t="n">
-        <v>-58.479921</v>
-      </c>
-      <c r="N97" t="n">
-        <v>-34.673021</v>
-      </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P97" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>6372</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>7/8/2025</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>AVELLANEDA 4500</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>808099405</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I98" t="n">
-        <v>1</v>
-      </c>
-      <c r="J98" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M98" t="n">
-        <v>-58.489219</v>
-      </c>
-      <c r="N98" t="n">
-        <v>-34.632475</v>
-      </c>
-      <c r="O98" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P98" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>